<commit_message>
anexando proceso para consolidar los recaudos descargados en un archivo excel
</commit_message>
<xml_diff>
--- a/Data/cuentas.xlsx
+++ b/Data/cuentas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpumarej\Documents\UiPath\Consolidacion de Recaudo\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpumarej\Documents\UiPath\Consolidacion de recaudos por caja\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9285D4A0-0FFA-4365-8135-A30DB5C01A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B952567E-82FD-4B38-B712-B84548A72D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informe" sheetId="3" r:id="rId1"/>
@@ -902,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -984,9 +984,27 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -999,24 +1017,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1027,6 +1027,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1346,7 +1352,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1380,87 +1386,87 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="C2" s="14">
-        <v>160</v>
+        <v>905</v>
       </c>
       <c r="D2" s="14">
-        <v>160</v>
+        <v>502</v>
       </c>
       <c r="E2" s="14">
-        <v>161</v>
+        <v>14</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G2" s="35"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C3" s="14">
-        <v>404</v>
+        <v>905</v>
       </c>
       <c r="D3" s="14">
-        <v>404</v>
+        <v>23</v>
       </c>
       <c r="E3" s="14">
-        <v>404</v>
+        <v>125</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="G3" s="35"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>109</v>
+        <v>6</v>
       </c>
       <c r="C4" s="14">
-        <v>905</v>
+        <v>160</v>
       </c>
       <c r="D4" s="14">
-        <v>502</v>
+        <v>160</v>
       </c>
       <c r="E4" s="14">
-        <v>14</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="G4" s="35"/>
+        <v>161</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="53"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" s="14">
-        <v>905</v>
+        <v>404</v>
       </c>
       <c r="D5" s="14">
-        <v>23</v>
+        <v>404</v>
       </c>
       <c r="E5" s="14">
-        <v>125</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>147</v>
-      </c>
-      <c r="G5" s="35"/>
+        <v>404</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="53"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
@@ -1716,23 +1722,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1775,10 +1781,10 @@
       <c r="E2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="45"/>
+      <c r="G2" s="38"/>
     </row>
     <row r="3" spans="3:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C3" s="22">
@@ -1790,10 +1796,10 @@
       <c r="E3" s="23">
         <v>110</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="G3" s="47"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="3:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C4" s="22">
@@ -1805,10 +1811,10 @@
       <c r="E4" s="23">
         <v>111</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="47"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="3:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="22">
@@ -1820,10 +1826,10 @@
       <c r="E5" s="23">
         <v>112</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="47"/>
+      <c r="G5" s="40"/>
     </row>
     <row r="6" spans="3:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C6" s="22">
@@ -1835,20 +1841,20 @@
       <c r="E6" s="23">
         <v>113</v>
       </c>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="47"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" spans="3:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C8" s="16" t="s">
@@ -1863,10 +1869,10 @@
       <c r="F8" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="42" t="s">
+      <c r="G8" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="42"/>
+      <c r="H8" s="43"/>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C9" s="16" t="s">
@@ -1881,10 +1887,10 @@
       <c r="F9" s="14">
         <v>120</v>
       </c>
-      <c r="G9" s="37" t="s">
+      <c r="G9" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="H9" s="37"/>
+      <c r="H9" s="41"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C10" s="16" t="s">
@@ -1899,10 +1905,10 @@
       <c r="F10" s="14">
         <v>124</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="H10" s="37"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C11" s="16" t="s">
@@ -1917,10 +1923,10 @@
       <c r="F11" s="14">
         <v>143</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="H11" s="37"/>
+      <c r="H11" s="41"/>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C12" s="16" t="s">
@@ -1935,10 +1941,10 @@
       <c r="F12" s="14">
         <v>153</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="H12" s="37"/>
+      <c r="H12" s="41"/>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C13" s="16" t="s">
@@ -1953,10 +1959,10 @@
       <c r="F13" s="14">
         <v>141</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="H13" s="37"/>
+      <c r="H13" s="41"/>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C14" s="16" t="s">
@@ -1971,10 +1977,10 @@
       <c r="F14" s="14">
         <v>144</v>
       </c>
-      <c r="G14" s="37" t="s">
+      <c r="G14" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="H14" s="37"/>
+      <c r="H14" s="41"/>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C15" s="16" t="s">
@@ -1989,10 +1995,10 @@
       <c r="F15" s="14">
         <v>145</v>
       </c>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="H15" s="37"/>
+      <c r="H15" s="41"/>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C16" s="16" t="s">
@@ -2007,10 +2013,10 @@
       <c r="F16" s="14">
         <v>150</v>
       </c>
-      <c r="G16" s="37" t="s">
+      <c r="G16" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="H16" s="37"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C17" s="16" t="s">
@@ -2025,10 +2031,10 @@
       <c r="F17" s="14">
         <v>140</v>
       </c>
-      <c r="G17" s="37" t="s">
+      <c r="G17" s="41" t="s">
         <v>155</v>
       </c>
-      <c r="H17" s="37"/>
+      <c r="H17" s="41"/>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C18" s="16" t="s">
@@ -2043,10 +2049,10 @@
       <c r="F18" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="G18" s="37" t="s">
+      <c r="G18" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="H18" s="37"/>
+      <c r="H18" s="41"/>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C19" s="16" t="s">
@@ -2061,10 +2067,10 @@
       <c r="F19" s="14">
         <v>136</v>
       </c>
-      <c r="G19" s="37" t="s">
+      <c r="G19" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="H19" s="37"/>
+      <c r="H19" s="41"/>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C20" s="16" t="s">
@@ -2079,10 +2085,10 @@
       <c r="F20" s="14">
         <v>192</v>
       </c>
-      <c r="G20" s="37" t="s">
+      <c r="G20" s="41" t="s">
         <v>139</v>
       </c>
-      <c r="H20" s="37"/>
+      <c r="H20" s="41"/>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C21" s="16" t="s">
@@ -2097,10 +2103,10 @@
       <c r="F21" s="14">
         <v>100</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="H21" s="37"/>
+      <c r="H21" s="41"/>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C22" s="16" t="s">
@@ -2115,10 +2121,10 @@
       <c r="F22" s="14">
         <v>106</v>
       </c>
-      <c r="G22" s="37" t="s">
+      <c r="G22" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="H22" s="37"/>
+      <c r="H22" s="41"/>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C23" s="16" t="s">
@@ -2133,10 +2139,10 @@
       <c r="F23" s="14">
         <v>17</v>
       </c>
-      <c r="G23" s="37" t="s">
+      <c r="G23" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="H23" s="37"/>
+      <c r="H23" s="41"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C24" s="16" t="s">
@@ -2151,10 +2157,10 @@
       <c r="F24" s="14">
         <v>160</v>
       </c>
-      <c r="G24" s="37" t="s">
+      <c r="G24" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="H24" s="37"/>
+      <c r="H24" s="41"/>
     </row>
     <row r="25" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="16" t="s">
@@ -2169,10 +2175,10 @@
       <c r="F25" s="14">
         <v>175</v>
       </c>
-      <c r="G25" s="37" t="s">
+      <c r="G25" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="H25" s="37"/>
+      <c r="H25" s="41"/>
       <c r="L25" s="11"/>
     </row>
     <row r="26" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2188,10 +2194,10 @@
       <c r="F26" s="14">
         <v>177</v>
       </c>
-      <c r="G26" s="37" t="s">
+      <c r="G26" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="H26" s="37"/>
+      <c r="H26" s="41"/>
       <c r="L26" s="11"/>
     </row>
     <row r="27" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2207,10 +2213,10 @@
       <c r="F27" s="14">
         <v>185</v>
       </c>
-      <c r="G27" s="37" t="s">
+      <c r="G27" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="H27" s="37"/>
+      <c r="H27" s="41"/>
       <c r="L27" s="11"/>
     </row>
     <row r="28" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2226,10 +2232,10 @@
       <c r="F28" s="14">
         <v>878</v>
       </c>
-      <c r="G28" s="37" t="s">
+      <c r="G28" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="H28" s="37"/>
+      <c r="H28" s="41"/>
     </row>
     <row r="29" spans="3:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C29" s="16" t="s">
@@ -2244,10 +2250,10 @@
       <c r="F29" s="14">
         <v>154</v>
       </c>
-      <c r="G29" s="37" t="s">
+      <c r="G29" s="41" t="s">
         <v>146</v>
       </c>
-      <c r="H29" s="37"/>
+      <c r="H29" s="41"/>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C30" s="30" t="s">
@@ -2262,10 +2268,10 @@
       <c r="F30" s="14">
         <v>161</v>
       </c>
-      <c r="G30" s="37" t="s">
+      <c r="G30" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="H30" s="37"/>
+      <c r="H30" s="41"/>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C31" s="30" t="s">
@@ -2280,10 +2286,10 @@
       <c r="F31" s="14">
         <v>404</v>
       </c>
-      <c r="G31" s="37" t="s">
+      <c r="G31" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="H31" s="37"/>
+      <c r="H31" s="41"/>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C32" s="30" t="s">
@@ -2298,10 +2304,10 @@
       <c r="F32" s="14">
         <v>14</v>
       </c>
-      <c r="G32" s="37" t="s">
+      <c r="G32" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="H32" s="37"/>
+      <c r="H32" s="41"/>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C33" s="30" t="s">
@@ -2316,10 +2322,10 @@
       <c r="F33" s="14">
         <v>125</v>
       </c>
-      <c r="G33" s="37" t="s">
+      <c r="G33" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="H33" s="37"/>
+      <c r="H33" s="41"/>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C34" s="30" t="s">
@@ -2334,10 +2340,10 @@
       <c r="F34" s="14">
         <v>164</v>
       </c>
-      <c r="G34" s="37" t="s">
+      <c r="G34" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="H34" s="37"/>
+      <c r="H34" s="41"/>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C35" s="30" t="s">
@@ -2352,10 +2358,10 @@
       <c r="F35" s="14">
         <v>186</v>
       </c>
-      <c r="G35" s="37" t="s">
+      <c r="G35" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="H35" s="37"/>
+      <c r="H35" s="41"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C36" s="30" t="s">
@@ -2370,10 +2376,10 @@
       <c r="F36" s="14">
         <v>811</v>
       </c>
-      <c r="G36" s="37" t="s">
+      <c r="G36" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="H36" s="37"/>
+      <c r="H36" s="41"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C37" s="30" t="s">
@@ -2388,10 +2394,10 @@
       <c r="F37" s="14">
         <v>863</v>
       </c>
-      <c r="G37" s="37" t="s">
+      <c r="G37" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="H37" s="37"/>
+      <c r="H37" s="41"/>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C38" s="16" t="s">
@@ -2406,10 +2412,10 @@
       <c r="F38" s="14">
         <v>123</v>
       </c>
-      <c r="G38" s="37" t="s">
+      <c r="G38" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="H38" s="37"/>
+      <c r="H38" s="41"/>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C39" s="30" t="s">
@@ -2424,10 +2430,10 @@
       <c r="F39" s="14">
         <v>11</v>
       </c>
-      <c r="G39" s="37" t="s">
+      <c r="G39" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="H39" s="37"/>
+      <c r="H39" s="41"/>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C40" s="30" t="s">
@@ -2442,10 +2448,10 @@
       <c r="F40" s="14">
         <v>176</v>
       </c>
-      <c r="G40" s="37" t="s">
+      <c r="G40" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="H40" s="37"/>
+      <c r="H40" s="41"/>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C41" s="30" t="s">
@@ -2460,10 +2466,10 @@
       <c r="F41" s="14">
         <v>861</v>
       </c>
-      <c r="G41" s="37" t="s">
+      <c r="G41" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="H41" s="37"/>
+      <c r="H41" s="41"/>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C42" s="16" t="s">
@@ -2478,10 +2484,10 @@
       <c r="F42" s="14">
         <v>210</v>
       </c>
-      <c r="G42" s="37" t="s">
+      <c r="G42" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="H42" s="37"/>
+      <c r="H42" s="41"/>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C43" s="16" t="s">
@@ -2496,10 +2502,10 @@
       <c r="F43" s="14">
         <v>210</v>
       </c>
-      <c r="G43" s="37" t="s">
+      <c r="G43" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="H43" s="37"/>
+      <c r="H43" s="41"/>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C44" s="16" t="s">
@@ -2514,10 +2520,10 @@
       <c r="F44" s="14">
         <v>210</v>
       </c>
-      <c r="G44" s="37" t="s">
+      <c r="G44" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="H44" s="37"/>
+      <c r="H44" s="41"/>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C45" s="16" t="s">
@@ -2532,10 +2538,10 @@
       <c r="F45" s="14">
         <v>210</v>
       </c>
-      <c r="G45" s="37" t="s">
+      <c r="G45" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="H45" s="37"/>
+      <c r="H45" s="41"/>
     </row>
     <row r="46" spans="3:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="C46" s="16" t="s">
@@ -2550,10 +2556,10 @@
       <c r="F46" s="14">
         <v>210</v>
       </c>
-      <c r="G46" s="37">
+      <c r="G46" s="41">
         <v>24003948037</v>
       </c>
-      <c r="H46" s="37"/>
+      <c r="H46" s="41"/>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C47" s="16" t="s">
@@ -2568,10 +2574,10 @@
       <c r="F47" s="14">
         <v>240</v>
       </c>
-      <c r="G47" s="37" t="s">
+      <c r="G47" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="H47" s="37"/>
+      <c r="H47" s="41"/>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C48" s="30" t="s">
@@ -2586,10 +2592,10 @@
       <c r="F48" s="14">
         <v>601</v>
       </c>
-      <c r="G48" s="37" t="s">
+      <c r="G48" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="H48" s="37"/>
+      <c r="H48" s="41"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C49" s="30" t="s">
@@ -2604,10 +2610,10 @@
       <c r="F49" s="14">
         <v>606</v>
       </c>
-      <c r="G49" s="37" t="s">
+      <c r="G49" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="H49" s="37"/>
+      <c r="H49" s="41"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C50" s="30" t="s">
@@ -2622,10 +2628,10 @@
       <c r="F50" s="14">
         <v>608</v>
       </c>
-      <c r="G50" s="37" t="s">
+      <c r="G50" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="H50" s="37"/>
+      <c r="H50" s="41"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C51" s="30" t="s">
@@ -2640,10 +2646,10 @@
       <c r="F51" s="14">
         <v>860</v>
       </c>
-      <c r="G51" s="37" t="s">
+      <c r="G51" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="H51" s="37"/>
+      <c r="H51" s="41"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C52" s="16" t="s">
@@ -2658,10 +2664,10 @@
       <c r="F52" s="14">
         <v>870</v>
       </c>
-      <c r="G52" s="37" t="s">
+      <c r="G52" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="H52" s="37"/>
+      <c r="H52" s="41"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C53" s="30" t="s">
@@ -2676,10 +2682,10 @@
       <c r="F53" s="14">
         <v>877</v>
       </c>
-      <c r="G53" s="37" t="s">
+      <c r="G53" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="H53" s="37"/>
+      <c r="H53" s="41"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C54" s="16" t="s">
@@ -2694,10 +2700,10 @@
       <c r="F54" s="14">
         <v>879</v>
       </c>
-      <c r="G54" s="37" t="s">
+      <c r="G54" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="H54" s="37"/>
+      <c r="H54" s="41"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C55" s="16" t="s">
@@ -2712,10 +2718,10 @@
       <c r="F55" s="14">
         <v>177</v>
       </c>
-      <c r="G55" s="37" t="s">
+      <c r="G55" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="H55" s="37"/>
+      <c r="H55" s="41"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D56" s="19"/>
@@ -2723,14 +2729,14 @@
       <c r="G56" s="19"/>
     </row>
     <row r="57" spans="2:8" ht="21" x14ac:dyDescent="0.5">
-      <c r="C57" s="43" t="s">
+      <c r="C57" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="42"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B58" s="10">
@@ -2848,11 +2854,11 @@
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="C63" s="41"/>
-      <c r="D63" s="41"/>
-      <c r="E63" s="41"/>
-      <c r="F63" s="41"/>
-      <c r="G63" s="41"/>
+      <c r="C63" s="47"/>
+      <c r="D63" s="47"/>
+      <c r="E63" s="47"/>
+      <c r="F63" s="47"/>
+      <c r="G63" s="47"/>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C64" s="16" t="s">
@@ -2867,8 +2873,8 @@
       <c r="F64" s="14">
         <v>13</v>
       </c>
-      <c r="G64" s="39"/>
-      <c r="H64" s="40"/>
+      <c r="G64" s="45"/>
+      <c r="H64" s="46"/>
     </row>
     <row r="65" spans="3:8" ht="27.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C65" s="16" t="s">
@@ -2883,8 +2889,8 @@
       <c r="F65" s="14">
         <v>20</v>
       </c>
-      <c r="G65" s="39"/>
-      <c r="H65" s="40"/>
+      <c r="G65" s="45"/>
+      <c r="H65" s="46"/>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C66" s="16" t="s">
@@ -2899,8 +2905,8 @@
       <c r="F66" s="14">
         <v>58</v>
       </c>
-      <c r="G66" s="38"/>
-      <c r="H66" s="38"/>
+      <c r="G66" s="44"/>
+      <c r="H66" s="44"/>
     </row>
     <row r="67" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C67" s="16" t="s">
@@ -2915,8 +2921,8 @@
       <c r="F67" s="14">
         <v>99</v>
       </c>
-      <c r="G67" s="38"/>
-      <c r="H67" s="38"/>
+      <c r="G67" s="44"/>
+      <c r="H67" s="44"/>
     </row>
     <row r="68" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C68" s="16" t="s">
@@ -2931,8 +2937,8 @@
       <c r="F68" s="14">
         <v>5</v>
       </c>
-      <c r="G68" s="38"/>
-      <c r="H68" s="38"/>
+      <c r="G68" s="44"/>
+      <c r="H68" s="44"/>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C69" s="27"/>
@@ -2979,17 +2985,40 @@
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G30:H30"/>
@@ -3006,40 +3035,17 @@
     <mergeCell ref="G35:H35"/>
     <mergeCell ref="G36:H36"/>
     <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>